<commit_message>
Data edit salaries course
</commit_message>
<xml_diff>
--- a/assets/data/intro-data-j/teacher-salaries.xlsx
+++ b/assets/data/intro-data-j/teacher-salaries.xlsx
@@ -1,17 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27211"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierreforcioli-conti/cjworkbench/assets/data/intro-data-j/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1 - teacher-salaries" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1 - teacher-salaries" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>teacher-salaries</t>
   </si>
@@ -19,18 +35,17 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Average salary (not adjusted)</t>
+    <t>Average salary</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="&quot;$&quot;#,##0.00"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -42,7 +57,7 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
@@ -153,63 +168,119 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="FFDBDBDB"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -408,7 +479,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -427,7 +498,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -457,7 +528,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -483,7 +554,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -509,7 +580,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -535,7 +606,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -561,7 +632,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -587,7 +658,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -613,7 +684,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -639,7 +710,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -665,7 +736,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -678,9 +749,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -697,7 +774,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -716,7 +793,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -742,7 +819,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -768,7 +845,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -794,7 +871,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -820,7 +897,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -846,7 +923,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -872,7 +949,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -898,7 +975,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -924,7 +1001,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -950,7 +1027,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -963,9 +1040,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -979,7 +1062,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -998,7 +1081,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1028,7 +1111,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1054,7 +1137,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1080,7 +1163,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1106,7 +1189,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1132,7 +1215,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1158,7 +1241,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1184,7 +1267,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1210,7 +1293,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1236,7 +1319,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1249,91 +1332,100 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:B8"/>
+  <dimension ref="A1:IV8"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.17188" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.6719" style="1" customWidth="1"/>
-    <col min="3" max="256" width="8.35156" style="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.6640625" style="1" customWidth="1"/>
+    <col min="3" max="256" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="27.65" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
+      <c r="B1" s="7"/>
     </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="2" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" ht="20.25" customHeight="1">
-      <c r="A3" s="4">
+    <row r="3" spans="1:2" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3">
         <v>1969</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>8626</v>
       </c>
     </row>
-    <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="6">
+    <row r="4" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="5">
         <v>1979</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="6">
         <v>15970</v>
       </c>
     </row>
-    <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="6">
+    <row r="5" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="5">
         <v>1989</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="6">
         <v>31367</v>
       </c>
     </row>
-    <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="6">
+    <row r="6" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="5">
         <v>1999</v>
       </c>
-      <c r="B6" s="7">
+      <c r="B6" s="6">
         <v>41807</v>
       </c>
     </row>
-    <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="6">
+    <row r="7" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="5">
         <v>2009</v>
       </c>
-      <c r="B7" s="7">
+      <c r="B7" s="6">
         <v>55202</v>
       </c>
     </row>
-    <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="6">
+    <row r="8" spans="1:2" ht="20" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="5">
         <v>2016</v>
       </c>
-      <c r="B8" s="7">
+      <c r="B8" s="6">
         <v>58950</v>
       </c>
     </row>
@@ -1342,7 +1434,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>